<commit_message>
Flight crew scheduling: review fixes
</commit_message>
<xml_diff>
--- a/optaplanner-examples/data/flightcrewscheduling/unsolved/175flights-7days-Europe.xlsx
+++ b/optaplanner-examples/data/flightcrewscheduling/unsolved/175flights-7days-Europe.xlsx
@@ -6754,10 +6754,10 @@
       <c r="C3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="E3" s="3" t="s">
+      <c r="D3" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>74</v>
       </c>
       <c r="F3" s="3" t="s">
@@ -6885,7 +6885,7 @@
       <c r="D7" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="3" t="s">
         <v>74</v>
       </c>
       <c r="F7" s="2" t="s">
@@ -6894,10 +6894,10 @@
       <c r="G7" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="H7" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="I7" s="3" t="s">
+      <c r="H7" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="I7" s="2" t="s">
         <v>74</v>
       </c>
       <c r="J7" s="2" t="s">
@@ -7010,7 +7010,7 @@
       <c r="C11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="3" t="s">
         <v>74</v>
       </c>
       <c r="E11" s="2" t="s">
@@ -7019,10 +7019,10 @@
       <c r="F11" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="G11" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="H11" s="3" t="s">
+      <c r="G11" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="H11" s="2" t="s">
         <v>74</v>
       </c>
       <c r="I11" s="2" t="s">
@@ -7037,7 +7037,7 @@
         <v>92</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>18</v>
@@ -7057,7 +7057,7 @@
       <c r="H12" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="I12" s="2" t="s">
+      <c r="I12" s="3" t="s">
         <v>74</v>
       </c>
       <c r="J12" s="2" t="s">
@@ -7074,7 +7074,7 @@
       <c r="C13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="2" t="s">
         <v>74</v>
       </c>
       <c r="E13" s="2" t="s">
@@ -7086,13 +7086,13 @@
       <c r="G13" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="H13" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="J13" s="3" t="s">
+      <c r="H13" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="J13" s="2" t="s">
         <v>74</v>
       </c>
     </row>
@@ -7109,16 +7109,16 @@
       <c r="D14" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E14" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="F14" s="3" t="s">
+      <c r="E14" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>74</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="H14" s="3" t="s">
         <v>74</v>
       </c>
       <c r="I14" s="2" t="s">
@@ -7269,13 +7269,13 @@
       <c r="D19" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E19" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="G19" s="3" t="s">
+      <c r="E19" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="G19" s="2" t="s">
         <v>74</v>
       </c>
       <c r="H19" s="2" t="s">
@@ -7301,10 +7301,10 @@
       <c r="D20" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E20" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="F20" s="3" t="s">
+      <c r="E20" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F20" s="2" t="s">
         <v>74</v>
       </c>
       <c r="G20" s="2" t="s">
@@ -7316,7 +7316,7 @@
       <c r="I20" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="J20" s="3" t="s">
+      <c r="J20" s="2" t="s">
         <v>74</v>
       </c>
     </row>
@@ -7325,7 +7325,7 @@
         <v>101</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>18</v>
@@ -7345,10 +7345,10 @@
       <c r="H21" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="I21" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="J21" s="2" t="s">
+      <c r="I21" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="J21" s="3" t="s">
         <v>74</v>
       </c>
     </row>
@@ -7389,7 +7389,7 @@
         <v>103</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>17</v>
@@ -7467,16 +7467,16 @@
       <c r="F25" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="G25" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="H25" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="I25" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="J25" s="3" t="s">
+      <c r="G25" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="J25" s="2" t="s">
         <v>74</v>
       </c>
     </row>
@@ -7490,7 +7490,7 @@
       <c r="C26" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="D26" s="2" t="s">
         <v>74</v>
       </c>
       <c r="E26" s="2" t="s">
@@ -7499,7 +7499,7 @@
       <c r="F26" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="G26" s="3" t="s">
+      <c r="G26" s="2" t="s">
         <v>74</v>
       </c>
       <c r="H26" s="2" t="s">
@@ -7517,7 +7517,7 @@
         <v>107</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>18</v>
@@ -7549,7 +7549,7 @@
         <v>108</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>17</v>
@@ -7677,7 +7677,7 @@
         <v>112</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>18</v>
@@ -7685,10 +7685,10 @@
       <c r="D32" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E32" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="F32" s="3" t="s">
+      <c r="E32" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F32" s="2" t="s">
         <v>74</v>
       </c>
       <c r="G32" s="2" t="s">
@@ -7709,7 +7709,7 @@
         <v>113</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>17</v>
@@ -7726,10 +7726,10 @@
       <c r="G33" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="H33" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="I33" s="3" t="s">
+      <c r="H33" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="I33" s="2" t="s">
         <v>74</v>
       </c>
       <c r="J33" s="2" t="s">
@@ -7741,7 +7741,7 @@
         <v>114</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>17</v>
@@ -7778,7 +7778,7 @@
       <c r="C35" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="D35" s="2" t="s">
         <v>74</v>
       </c>
       <c r="E35" s="2" t="s">
@@ -7796,7 +7796,7 @@
       <c r="I35" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="J35" s="3" t="s">
+      <c r="J35" s="2" t="s">
         <v>74</v>
       </c>
     </row>
@@ -7805,7 +7805,7 @@
         <v>116</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>18</v>
@@ -7819,7 +7819,7 @@
       <c r="F36" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="G36" s="2" t="s">
+      <c r="G36" s="3" t="s">
         <v>74</v>
       </c>
       <c r="H36" s="2" t="s">
@@ -7877,7 +7877,7 @@
       <c r="D38" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E38" s="3" t="s">
+      <c r="E38" s="2" t="s">
         <v>74</v>
       </c>
       <c r="F38" s="2" t="s">
@@ -7886,7 +7886,7 @@
       <c r="G38" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="H38" s="3" t="s">
+      <c r="H38" s="2" t="s">
         <v>74</v>
       </c>
       <c r="I38" s="2" t="s">
@@ -7901,7 +7901,7 @@
         <v>119</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>17</v>
@@ -7933,7 +7933,7 @@
         <v>120</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>18</v>
@@ -7965,7 +7965,7 @@
         <v>121</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>18</v>
@@ -7985,7 +7985,7 @@
       <c r="H41" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="I41" s="2" t="s">
+      <c r="I41" s="3" t="s">
         <v>74</v>
       </c>
       <c r="J41" s="2" t="s">
@@ -8029,7 +8029,7 @@
         <v>123</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>17</v>
@@ -8040,16 +8040,16 @@
       <c r="E43" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="F43" s="3" t="s">
+      <c r="F43" s="2" t="s">
         <v>74</v>
       </c>
       <c r="G43" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="H43" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="I43" s="3" t="s">
+      <c r="H43" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="I43" s="2" t="s">
         <v>74</v>
       </c>
       <c r="J43" s="2" t="s">
@@ -8061,7 +8061,7 @@
         <v>124</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>17</v>
@@ -8093,27 +8093,27 @@
         <v>125</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D45" s="2" t="s">
+      <c r="D45" s="3" t="s">
         <v>74</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="F45" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="G45" s="3" t="s">
+      <c r="F45" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G45" s="2" t="s">
         <v>74</v>
       </c>
       <c r="H45" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="I45" s="3" t="s">
+      <c r="I45" s="2" t="s">
         <v>74</v>
       </c>
       <c r="J45" s="2" t="s">
@@ -8125,7 +8125,7 @@
         <v>126</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>18</v>
@@ -8157,7 +8157,7 @@
         <v>127</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>18</v>
@@ -8165,7 +8165,7 @@
       <c r="D47" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E47" s="3" t="s">
+      <c r="E47" s="2" t="s">
         <v>74</v>
       </c>
       <c r="F47" s="2" t="s">
@@ -8180,7 +8180,7 @@
       <c r="I47" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="J47" s="3" t="s">
+      <c r="J47" s="2" t="s">
         <v>74</v>
       </c>
     </row>
@@ -8189,7 +8189,7 @@
         <v>128</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>17</v>
@@ -8221,7 +8221,7 @@
         <v>129</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>17</v>
@@ -8253,7 +8253,7 @@
         <v>130</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>18</v>
@@ -8317,24 +8317,24 @@
         <v>132</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D52" s="3" t="s">
+      <c r="D52" s="2" t="s">
         <v>74</v>
       </c>
       <c r="E52" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="F52" s="2" t="s">
+      <c r="F52" s="3" t="s">
         <v>74</v>
       </c>
       <c r="G52" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="H52" s="3" t="s">
+      <c r="H52" s="2" t="s">
         <v>74</v>
       </c>
       <c r="I52" s="2" t="s">
@@ -8363,7 +8363,7 @@
       <c r="F53" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="G53" s="3" t="s">
+      <c r="G53" s="2" t="s">
         <v>74</v>
       </c>
       <c r="H53" s="2" t="s">
@@ -8381,7 +8381,7 @@
         <v>134</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>17</v>
@@ -8404,7 +8404,7 @@
       <c r="I54" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="J54" s="2" t="s">
+      <c r="J54" s="3" t="s">
         <v>74</v>
       </c>
     </row>
@@ -8418,25 +8418,25 @@
       <c r="C55" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D55" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="F55" s="3" t="s">
+      <c r="D55" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F55" s="2" t="s">
         <v>74</v>
       </c>
       <c r="G55" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="H55" s="3" t="s">
+      <c r="H55" s="2" t="s">
         <v>74</v>
       </c>
       <c r="I55" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="J55" s="3" t="s">
+      <c r="J55" s="2" t="s">
         <v>74</v>
       </c>
     </row>
@@ -8477,7 +8477,7 @@
         <v>137</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>18</v>
@@ -8532,7 +8532,7 @@
       <c r="I58" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="J58" s="2" t="s">
+      <c r="J58" s="3" t="s">
         <v>74</v>
       </c>
     </row>
@@ -8541,7 +8541,7 @@
         <v>139</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>17</v>
@@ -8573,7 +8573,7 @@
         <v>140</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>18</v>
@@ -8637,7 +8637,7 @@
         <v>142</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>18</v>
@@ -8654,7 +8654,7 @@
       <c r="G62" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="H62" s="2" t="s">
+      <c r="H62" s="3" t="s">
         <v>74</v>
       </c>
       <c r="I62" s="2" t="s">
@@ -8669,7 +8669,7 @@
         <v>143</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>17</v>
@@ -8683,13 +8683,13 @@
       <c r="F63" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="G63" s="3" t="s">
+      <c r="G63" s="2" t="s">
         <v>74</v>
       </c>
       <c r="H63" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="I63" s="3" t="s">
+      <c r="I63" s="2" t="s">
         <v>74</v>
       </c>
       <c r="J63" s="2" t="s">
@@ -8718,10 +8718,10 @@
       <c r="G64" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="H64" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="I64" s="3" t="s">
+      <c r="H64" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="I64" s="2" t="s">
         <v>74</v>
       </c>
       <c r="J64" s="2" t="s">
@@ -8738,7 +8738,7 @@
       <c r="C65" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D65" s="2" t="s">
+      <c r="D65" s="3" t="s">
         <v>74</v>
       </c>
       <c r="E65" s="2" t="s">
@@ -8747,7 +8747,7 @@
       <c r="F65" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="G65" s="2" t="s">
+      <c r="G65" s="3" t="s">
         <v>74</v>
       </c>
       <c r="H65" s="2" t="s">
@@ -8765,7 +8765,7 @@
         <v>146</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>18</v>
@@ -8776,7 +8776,7 @@
       <c r="E66" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="F66" s="2" t="s">
+      <c r="F66" s="3" t="s">
         <v>74</v>
       </c>
       <c r="G66" s="2" t="s">
@@ -8802,7 +8802,7 @@
       <c r="C67" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D67" s="3" t="s">
+      <c r="D67" s="2" t="s">
         <v>74</v>
       </c>
       <c r="E67" s="2" t="s">
@@ -8820,7 +8820,7 @@
       <c r="I67" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="J67" s="3" t="s">
+      <c r="J67" s="2" t="s">
         <v>74</v>
       </c>
     </row>
@@ -8829,7 +8829,7 @@
         <v>148</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>17</v>
@@ -8869,10 +8869,10 @@
       <c r="D69" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E69" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="F69" s="3" t="s">
+      <c r="E69" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F69" s="2" t="s">
         <v>74</v>
       </c>
       <c r="G69" s="2" t="s">
@@ -8881,7 +8881,7 @@
       <c r="H69" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="I69" s="2" t="s">
+      <c r="I69" s="3" t="s">
         <v>74</v>
       </c>
       <c r="J69" s="2" t="s">
@@ -8893,7 +8893,7 @@
         <v>150</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>18</v>
@@ -8901,7 +8901,7 @@
       <c r="D70" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E70" s="3" t="s">
+      <c r="E70" s="2" t="s">
         <v>74</v>
       </c>
       <c r="F70" s="2" t="s">
@@ -8916,7 +8916,7 @@
       <c r="I70" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="J70" s="3" t="s">
+      <c r="J70" s="2" t="s">
         <v>74</v>
       </c>
     </row>
@@ -8930,22 +8930,22 @@
       <c r="C71" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D71" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="E71" s="2" t="s">
+      <c r="D71" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E71" s="3" t="s">
         <v>74</v>
       </c>
       <c r="F71" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="G71" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="H71" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="I71" s="3" t="s">
+      <c r="G71" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="H71" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="I71" s="2" t="s">
         <v>74</v>
       </c>
       <c r="J71" s="2" t="s">
@@ -8957,7 +8957,7 @@
         <v>152</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C72" s="2" t="s">
         <v>18</v>
@@ -8989,30 +8989,30 @@
         <v>153</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C73" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D73" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="E73" s="3" t="s">
+      <c r="D73" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E73" s="2" t="s">
         <v>74</v>
       </c>
       <c r="F73" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="G73" s="3" t="s">
+      <c r="G73" s="2" t="s">
         <v>74</v>
       </c>
       <c r="H73" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="I73" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="J73" s="3" t="s">
+      <c r="I73" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="J73" s="2" t="s">
         <v>74</v>
       </c>
     </row>
@@ -9076,7 +9076,7 @@
       <c r="I75" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="J75" s="2" t="s">
+      <c r="J75" s="3" t="s">
         <v>74</v>
       </c>
     </row>
@@ -9085,7 +9085,7 @@
         <v>156</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C76" s="2" t="s">
         <v>18</v>
@@ -9096,13 +9096,13 @@
       <c r="E76" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="F76" s="3" t="s">
+      <c r="F76" s="2" t="s">
         <v>74</v>
       </c>
       <c r="G76" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="H76" s="3" t="s">
+      <c r="H76" s="2" t="s">
         <v>74</v>
       </c>
       <c r="I76" s="2" t="s">
@@ -9117,7 +9117,7 @@
         <v>157</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C77" s="2" t="s">
         <v>18</v>
@@ -9149,12 +9149,12 @@
         <v>158</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C78" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D78" s="2" t="s">
+      <c r="D78" s="3" t="s">
         <v>74</v>
       </c>
       <c r="E78" s="2" t="s">
@@ -9181,7 +9181,7 @@
         <v>159</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C79" s="2" t="s">
         <v>17</v>
@@ -9213,7 +9213,7 @@
         <v>160</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C80" s="2" t="s">
         <v>18</v>
@@ -9245,7 +9245,7 @@
         <v>161</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C81" s="2" t="s">
         <v>18</v>
@@ -9253,7 +9253,7 @@
       <c r="D81" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E81" s="3" t="s">
+      <c r="E81" s="2" t="s">
         <v>74</v>
       </c>
       <c r="F81" s="2" t="s">
@@ -9265,7 +9265,7 @@
       <c r="H81" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="I81" s="3" t="s">
+      <c r="I81" s="2" t="s">
         <v>74</v>
       </c>
       <c r="J81" s="2" t="s">
@@ -9277,18 +9277,18 @@
         <v>162</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C82" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D82" s="3" t="s">
+      <c r="D82" s="2" t="s">
         <v>74</v>
       </c>
       <c r="E82" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="F82" s="3" t="s">
+      <c r="F82" s="2" t="s">
         <v>74</v>
       </c>
       <c r="G82" s="2" t="s">
@@ -9309,7 +9309,7 @@
         <v>163</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C83" s="2" t="s">
         <v>17</v>
@@ -9332,7 +9332,7 @@
       <c r="I83" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="J83" s="3" t="s">
+      <c r="J83" s="2" t="s">
         <v>74</v>
       </c>
     </row>
@@ -9341,7 +9341,7 @@
         <v>164</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C84" s="2" t="s">
         <v>17</v>
@@ -9373,12 +9373,12 @@
         <v>165</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C85" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D85" s="3" t="s">
+      <c r="D85" s="2" t="s">
         <v>74</v>
       </c>
       <c r="E85" s="2" t="s">
@@ -9419,7 +9419,7 @@
       <c r="F86" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="G86" s="2" t="s">
+      <c r="G86" s="3" t="s">
         <v>74</v>
       </c>
       <c r="H86" s="2" t="s">
@@ -9460,7 +9460,7 @@
       <c r="I87" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="J87" s="2" t="s">
+      <c r="J87" s="3" t="s">
         <v>74</v>
       </c>
     </row>
@@ -9477,22 +9477,22 @@
       <c r="D88" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E88" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="F88" s="3" t="s">
+      <c r="E88" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F88" s="2" t="s">
         <v>74</v>
       </c>
       <c r="G88" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="H88" s="3" t="s">
+      <c r="H88" s="2" t="s">
         <v>74</v>
       </c>
       <c r="I88" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="J88" s="3" t="s">
+      <c r="J88" s="2" t="s">
         <v>74</v>
       </c>
     </row>
@@ -9533,7 +9533,7 @@
         <v>170</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C90" s="2" t="s">
         <v>18</v>
@@ -9544,7 +9544,7 @@
       <c r="E90" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="F90" s="2" t="s">
+      <c r="F90" s="3" t="s">
         <v>74</v>
       </c>
       <c r="G90" s="2" t="s">
@@ -9570,13 +9570,13 @@
       <c r="C91" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D91" s="3" t="s">
+      <c r="D91" s="2" t="s">
         <v>74</v>
       </c>
       <c r="E91" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="F91" s="3" t="s">
+      <c r="F91" s="2" t="s">
         <v>74</v>
       </c>
       <c r="G91" s="2" t="s">
@@ -9597,7 +9597,7 @@
         <v>172</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C92" s="2" t="s">
         <v>18</v>
@@ -9605,7 +9605,7 @@
       <c r="D92" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E92" s="3" t="s">
+      <c r="E92" s="2" t="s">
         <v>74</v>
       </c>
       <c r="F92" s="2" t="s">
@@ -9614,10 +9614,10 @@
       <c r="G92" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="H92" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="I92" s="2" t="s">
+      <c r="H92" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="I92" s="3" t="s">
         <v>74</v>
       </c>
       <c r="J92" s="2" t="s">
@@ -9693,7 +9693,7 @@
         <v>175</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C95" s="2" t="s">
         <v>18</v>
@@ -9701,7 +9701,7 @@
       <c r="D95" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E95" s="2" t="s">
+      <c r="E95" s="3" t="s">
         <v>74</v>
       </c>
       <c r="F95" s="2" t="s">
@@ -9713,10 +9713,10 @@
       <c r="H95" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="I95" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="J95" s="3" t="s">
+      <c r="I95" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="J95" s="2" t="s">
         <v>74</v>
       </c>
     </row>
@@ -9725,7 +9725,7 @@
         <v>176</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C96" s="2" t="s">
         <v>18</v>
@@ -9757,7 +9757,7 @@
         <v>177</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C97" s="2" t="s">
         <v>18</v>
@@ -9774,7 +9774,7 @@
       <c r="G97" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="H97" s="2" t="s">
+      <c r="H97" s="3" t="s">
         <v>74</v>
       </c>
       <c r="I97" s="2" t="s">
@@ -9794,16 +9794,16 @@
       <c r="C98" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D98" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="E98" s="3" t="s">
+      <c r="D98" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E98" s="2" t="s">
         <v>74</v>
       </c>
       <c r="F98" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="G98" s="3" t="s">
+      <c r="G98" s="2" t="s">
         <v>74</v>
       </c>
       <c r="H98" s="2" t="s">
@@ -9821,7 +9821,7 @@
         <v>179</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C99" s="2" t="s">
         <v>17</v>
@@ -9832,7 +9832,7 @@
       <c r="E99" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="F99" s="3" t="s">
+      <c r="F99" s="2" t="s">
         <v>74</v>
       </c>
       <c r="G99" s="2" t="s">
@@ -9844,7 +9844,7 @@
       <c r="I99" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="J99" s="3" t="s">
+      <c r="J99" s="2" t="s">
         <v>74</v>
       </c>
     </row>
@@ -9861,7 +9861,7 @@
       <c r="D100" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E100" s="2" t="s">
+      <c r="E100" s="3" t="s">
         <v>74</v>
       </c>
       <c r="F100" s="2" t="s">
@@ -9917,7 +9917,7 @@
         <v>182</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C102" s="2" t="s">
         <v>18</v>
@@ -9940,7 +9940,7 @@
       <c r="I102" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="J102" s="2" t="s">
+      <c r="J102" s="3" t="s">
         <v>74</v>
       </c>
     </row>
@@ -9949,7 +9949,7 @@
         <v>183</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C103" s="2" t="s">
         <v>17</v>
@@ -9995,10 +9995,10 @@
       <c r="F104" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="G104" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="H104" s="3" t="s">
+      <c r="G104" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="H104" s="2" t="s">
         <v>74</v>
       </c>
       <c r="I104" s="2" t="s">
@@ -10013,7 +10013,7 @@
         <v>185</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C105" s="2" t="s">
         <v>18</v>
@@ -10088,7 +10088,7 @@
       <c r="E107" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="F107" s="2" t="s">
+      <c r="F107" s="3" t="s">
         <v>74</v>
       </c>
       <c r="G107" s="2" t="s">
@@ -10129,7 +10129,7 @@
       <c r="H108" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="I108" s="2" t="s">
+      <c r="I108" s="3" t="s">
         <v>74</v>
       </c>
       <c r="J108" s="2" t="s">
@@ -10173,7 +10173,7 @@
         <v>190</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C110" s="2" t="s">
         <v>18</v>
@@ -10205,12 +10205,12 @@
         <v>191</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C111" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D111" s="3" t="s">
+      <c r="D111" s="2" t="s">
         <v>74</v>
       </c>
       <c r="E111" s="2" t="s">
@@ -10225,7 +10225,7 @@
       <c r="H111" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="I111" s="3" t="s">
+      <c r="I111" s="2" t="s">
         <v>74</v>
       </c>
       <c r="J111" s="2" t="s">
@@ -10237,7 +10237,7 @@
         <v>192</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C112" s="2" t="s">
         <v>18</v>
@@ -10245,13 +10245,13 @@
       <c r="D112" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E112" s="3" t="s">
+      <c r="E112" s="2" t="s">
         <v>74</v>
       </c>
       <c r="F112" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="G112" s="3" t="s">
+      <c r="G112" s="2" t="s">
         <v>74</v>
       </c>
       <c r="H112" s="2" t="s">
@@ -10274,7 +10274,7 @@
       <c r="C113" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D113" s="2" t="s">
+      <c r="D113" s="3" t="s">
         <v>74</v>
       </c>
       <c r="E113" s="2" t="s">
@@ -10286,7 +10286,7 @@
       <c r="G113" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="H113" s="2" t="s">
+      <c r="H113" s="3" t="s">
         <v>74</v>
       </c>
       <c r="I113" s="2" t="s">
@@ -10365,7 +10365,7 @@
         <v>196</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C116" s="2" t="s">
         <v>18</v>
@@ -10434,22 +10434,22 @@
       <c r="C118" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D118" s="3" t="s">
+      <c r="D118" s="2" t="s">
         <v>74</v>
       </c>
       <c r="E118" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="F118" s="3" t="s">
+      <c r="F118" s="2" t="s">
         <v>74</v>
       </c>
       <c r="G118" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="H118" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="I118" s="3" t="s">
+      <c r="H118" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="I118" s="2" t="s">
         <v>74</v>
       </c>
       <c r="J118" s="2" t="s">
@@ -10461,7 +10461,7 @@
         <v>199</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C119" s="2" t="s">
         <v>17</v>
@@ -10525,12 +10525,12 @@
         <v>201</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C121" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D121" s="3" t="s">
+      <c r="D121" s="2" t="s">
         <v>74</v>
       </c>
       <c r="E121" s="2" t="s">
@@ -10548,7 +10548,7 @@
       <c r="I121" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="J121" s="3" t="s">
+      <c r="J121" s="2" t="s">
         <v>74</v>
       </c>
     </row>
@@ -10589,7 +10589,7 @@
         <v>203</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C123" s="2" t="s">
         <v>17</v>
@@ -10621,7 +10621,7 @@
         <v>204</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C124" s="2" t="s">
         <v>17</v>
@@ -10725,19 +10725,19 @@
       <c r="D127" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E127" s="3" t="s">
+      <c r="E127" s="2" t="s">
         <v>74</v>
       </c>
       <c r="F127" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="G127" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="H127" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="I127" s="3" t="s">
+      <c r="G127" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="H127" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="I127" s="2" t="s">
         <v>74</v>
       </c>
       <c r="J127" s="2" t="s">
@@ -10749,7 +10749,7 @@
         <v>208</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C128" s="2" t="s">
         <v>17</v>
@@ -10813,7 +10813,7 @@
         <v>210</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C130" s="2" t="s">
         <v>18</v>
@@ -10827,7 +10827,7 @@
       <c r="F130" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="G130" s="2" t="s">
+      <c r="G130" s="3" t="s">
         <v>74</v>
       </c>
       <c r="H130" s="2" t="s">
@@ -10845,7 +10845,7 @@
         <v>211</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C131" s="2" t="s">
         <v>18</v>
@@ -10856,7 +10856,7 @@
       <c r="E131" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="F131" s="3" t="s">
+      <c r="F131" s="2" t="s">
         <v>74</v>
       </c>
       <c r="G131" s="2" t="s">
@@ -10865,10 +10865,10 @@
       <c r="H131" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="I131" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="J131" s="3" t="s">
+      <c r="I131" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="J131" s="2" t="s">
         <v>74</v>
       </c>
     </row>
@@ -10877,7 +10877,7 @@
         <v>212</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C132" s="2" t="s">
         <v>18</v>
@@ -10885,7 +10885,7 @@
       <c r="D132" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E132" s="2" t="s">
+      <c r="E132" s="3" t="s">
         <v>74</v>
       </c>
       <c r="F132" s="2" t="s">
@@ -10909,7 +10909,7 @@
         <v>213</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C133" s="2" t="s">
         <v>17</v>
@@ -10978,10 +10978,10 @@
       <c r="C135" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D135" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="E135" s="3" t="s">
+      <c r="D135" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E135" s="2" t="s">
         <v>74</v>
       </c>
       <c r="F135" s="2" t="s">
@@ -10993,10 +10993,10 @@
       <c r="H135" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="I135" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="J135" s="3" t="s">
+      <c r="I135" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="J135" s="2" t="s">
         <v>74</v>
       </c>
     </row>
@@ -11019,10 +11019,10 @@
       <c r="F136" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="G136" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="H136" s="3" t="s">
+      <c r="G136" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="H136" s="2" t="s">
         <v>74</v>
       </c>
       <c r="I136" s="2" t="s">
@@ -11118,7 +11118,7 @@
       <c r="G139" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="H139" s="2" t="s">
+      <c r="H139" s="3" t="s">
         <v>74</v>
       </c>
       <c r="I139" s="2" t="s">
@@ -11133,18 +11133,18 @@
         <v>220</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C140" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D140" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="E140" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="F140" s="3" t="s">
+      <c r="D140" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E140" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F140" s="2" t="s">
         <v>74</v>
       </c>
       <c r="G140" s="2" t="s">
@@ -11176,7 +11176,7 @@
       <c r="E141" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="F141" s="2" t="s">
+      <c r="F141" s="3" t="s">
         <v>74</v>
       </c>
       <c r="G141" s="2" t="s">
@@ -11202,7 +11202,7 @@
       <c r="C142" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D142" s="3" t="s">
+      <c r="D142" s="2" t="s">
         <v>74</v>
       </c>
       <c r="E142" s="2" t="s">
@@ -11211,7 +11211,7 @@
       <c r="F142" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="G142" s="3" t="s">
+      <c r="G142" s="2" t="s">
         <v>74</v>
       </c>
       <c r="H142" s="2" t="s">
@@ -11293,7 +11293,7 @@
         <v>225</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C145" s="2" t="s">
         <v>18</v>
@@ -11348,7 +11348,7 @@
       <c r="I146" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="J146" s="2" t="s">
+      <c r="J146" s="3" t="s">
         <v>74</v>
       </c>
     </row>
@@ -11357,7 +11357,7 @@
         <v>227</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C147" s="2" t="s">
         <v>18</v>
@@ -11389,7 +11389,7 @@
         <v>228</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C148" s="2" t="s">
         <v>17</v>
@@ -11421,30 +11421,30 @@
         <v>229</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C149" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D149" s="3" t="s">
+      <c r="D149" s="2" t="s">
         <v>74</v>
       </c>
       <c r="E149" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="F149" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="G149" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="H149" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="I149" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="J149" s="3" t="s">
+      <c r="F149" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G149" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="H149" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="I149" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="J149" s="2" t="s">
         <v>74</v>
       </c>
     </row>
@@ -16457,7 +16457,7 @@
         <v>92</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13">
@@ -16529,7 +16529,7 @@
         <v>101</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22">
@@ -16545,7 +16545,7 @@
         <v>103</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24">
@@ -16577,7 +16577,7 @@
         <v>107</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28">
@@ -16585,7 +16585,7 @@
         <v>108</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="29">
@@ -16617,7 +16617,7 @@
         <v>112</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="33">
@@ -16625,7 +16625,7 @@
         <v>113</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="34">
@@ -16633,7 +16633,7 @@
         <v>114</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="35">
@@ -16649,7 +16649,7 @@
         <v>116</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="37">
@@ -16673,7 +16673,7 @@
         <v>119</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="40">
@@ -16681,7 +16681,7 @@
         <v>120</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="41">
@@ -16689,7 +16689,7 @@
         <v>121</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="42">
@@ -16705,7 +16705,7 @@
         <v>123</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="44">
@@ -16713,7 +16713,7 @@
         <v>124</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="45">
@@ -16721,7 +16721,7 @@
         <v>125</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="46">
@@ -16729,7 +16729,7 @@
         <v>126</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="47">
@@ -16737,7 +16737,7 @@
         <v>127</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="48">
@@ -16745,7 +16745,7 @@
         <v>128</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="49">
@@ -16753,7 +16753,7 @@
         <v>129</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="50">
@@ -16761,7 +16761,7 @@
         <v>130</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="51">
@@ -16777,7 +16777,7 @@
         <v>132</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="53">
@@ -16793,7 +16793,7 @@
         <v>134</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="55">
@@ -16817,7 +16817,7 @@
         <v>137</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="58">
@@ -16833,7 +16833,7 @@
         <v>139</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="60">
@@ -16841,7 +16841,7 @@
         <v>140</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="61">
@@ -16857,7 +16857,7 @@
         <v>142</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="63">
@@ -16865,7 +16865,7 @@
         <v>143</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="64">
@@ -16889,7 +16889,7 @@
         <v>146</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="67">
@@ -16905,7 +16905,7 @@
         <v>148</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="69">
@@ -16921,7 +16921,7 @@
         <v>150</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="71">
@@ -16937,7 +16937,7 @@
         <v>152</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="73">
@@ -16945,7 +16945,7 @@
         <v>153</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="74">
@@ -16969,7 +16969,7 @@
         <v>156</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="77">
@@ -16977,7 +16977,7 @@
         <v>157</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="78">
@@ -16985,7 +16985,7 @@
         <v>158</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="79">
@@ -16993,7 +16993,7 @@
         <v>159</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="80">
@@ -17001,7 +17001,7 @@
         <v>160</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="81">
@@ -17009,7 +17009,7 @@
         <v>161</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="82">
@@ -17017,7 +17017,7 @@
         <v>162</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="83">
@@ -17025,7 +17025,7 @@
         <v>163</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="84">
@@ -17033,7 +17033,7 @@
         <v>164</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="85">
@@ -17041,7 +17041,7 @@
         <v>165</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="86">
@@ -17081,7 +17081,7 @@
         <v>170</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="91">
@@ -17097,7 +17097,7 @@
         <v>172</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="93">
@@ -17121,7 +17121,7 @@
         <v>175</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="96">
@@ -17129,7 +17129,7 @@
         <v>176</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="97">
@@ -17137,7 +17137,7 @@
         <v>177</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="98">
@@ -17153,7 +17153,7 @@
         <v>179</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="100">
@@ -17177,7 +17177,7 @@
         <v>182</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="103">
@@ -17185,7 +17185,7 @@
         <v>183</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="104">
@@ -17201,7 +17201,7 @@
         <v>185</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="106">
@@ -17241,7 +17241,7 @@
         <v>190</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="111">
@@ -17249,7 +17249,7 @@
         <v>191</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="112">
@@ -17257,7 +17257,7 @@
         <v>192</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="113">
@@ -17289,7 +17289,7 @@
         <v>196</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="117">
@@ -17313,7 +17313,7 @@
         <v>199</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="120">
@@ -17329,7 +17329,7 @@
         <v>201</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="122">
@@ -17345,7 +17345,7 @@
         <v>203</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="124">
@@ -17353,7 +17353,7 @@
         <v>204</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="125">
@@ -17385,7 +17385,7 @@
         <v>208</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="129">
@@ -17401,7 +17401,7 @@
         <v>210</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="131">
@@ -17409,7 +17409,7 @@
         <v>211</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="132">
@@ -17417,7 +17417,7 @@
         <v>212</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="133">
@@ -17425,7 +17425,7 @@
         <v>213</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="134">
@@ -17481,7 +17481,7 @@
         <v>220</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="141">
@@ -17521,7 +17521,7 @@
         <v>225</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="146">
@@ -17537,7 +17537,7 @@
         <v>227</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="148">
@@ -17545,7 +17545,7 @@
         <v>228</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="149">
@@ -17553,7 +17553,7 @@
         <v>229</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="150">

</xml_diff>